<commit_message>
Sesuaikan semua year ke date
</commit_message>
<xml_diff>
--- a/public/import.xlsx
+++ b/public/import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Univ\Self\Belajar Laravel\Laravel 6\Project\inventaris\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E38D0E-5BE3-41CA-92A4-E9A26158767C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EED8CD8-728F-4188-A0E4-252A53D2937B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Lokasi</t>
   </si>
   <si>
-    <t>Tahun Pembelian</t>
-  </si>
-  <si>
     <t>Kondisi</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Tanggal Pembelian (DD-MM-YYYY)</t>
   </si>
 </sst>
 </file>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
     <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
@@ -452,22 +452,22 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>